<commit_message>
Updated Logger class and Program Delete Scenario
</commit_message>
<xml_diff>
--- a/src/test/java/com/api/testdata/DataExcel.xlsx
+++ b/src/test/java/com/api/testdata/DataExcel.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinth\eclipse-workspace\restapi\src\test\java\com\api\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinth\eclipse-workspace\NinjaSparks_API_Hackathon\src\test\java\com\api\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DDFA87-0A97-4557-9A6D-E6CBCC76331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A303E6D-9CA2-418B-AB0A-D1861C134148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{73EA3766-16BF-4183-83E6-A22A49A2E0C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{73EA3766-16BF-4183-83E6-A22A49A2E0C6}"/>
   </bookViews>
   <sheets>
-    <sheet name="postdata" sheetId="2" r:id="rId1"/>
-    <sheet name="putdata" sheetId="3" r:id="rId2"/>
-    <sheet name="putProgramname" sheetId="4" r:id="rId3"/>
+    <sheet name="create" sheetId="5" r:id="rId1"/>
+    <sheet name="postdata" sheetId="2" r:id="rId2"/>
+    <sheet name="putdata" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>programName</t>
   </si>
@@ -41,31 +41,34 @@
     <t>Active</t>
   </si>
   <si>
-    <t>API Testing</t>
-  </si>
-  <si>
-    <t>NinjaSparkCin001</t>
-  </si>
-  <si>
-    <t>NinjaSparkCin002</t>
-  </si>
-  <si>
     <t>NinjaSparkSDET1</t>
   </si>
   <si>
     <t>Learn API</t>
   </si>
   <si>
-    <t>NinjaSparkCin22</t>
-  </si>
-  <si>
-    <t>NinjaSparkCin23</t>
-  </si>
-  <si>
     <t>API Testing Eclipse</t>
   </si>
   <si>
     <t>API Testing cucumber</t>
+  </si>
+  <si>
+    <t>NinjaSparkCin221</t>
+  </si>
+  <si>
+    <t>NinjaSparkCin231</t>
+  </si>
+  <si>
+    <t>NinjaSparrree</t>
+  </si>
+  <si>
+    <t>NinjaDiiiee</t>
+  </si>
+  <si>
+    <t>Learn Automation</t>
+  </si>
+  <si>
+    <t>Learn API Test</t>
   </si>
 </sst>
 </file>
@@ -429,6 +432,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBF458C-3F05-453B-A50C-3F22DDDB678E}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D934DE-7C8E-4ABF-853C-4DAC70642562}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -469,10 +541,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -485,12 +557,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7933EB-B12C-4508-B919-C5C7CBB0B968}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,10 +585,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -524,10 +596,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -537,58 +609,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2505FE3C-C77E-4533-9B06-EE20BBBCF2B8}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated pom and program Feature
</commit_message>
<xml_diff>
--- a/src/test/java/com/api/testdata/DataExcel.xlsx
+++ b/src/test/java/com/api/testdata/DataExcel.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinth\eclipse-workspace\NinjaSparks_API_Hackathon\src\test\java\com\api\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A303E6D-9CA2-418B-AB0A-D1861C134148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C3D2BC-A750-42D4-99DA-5B84D4B05B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{73EA3766-16BF-4183-83E6-A22A49A2E0C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{73EA3766-16BF-4183-83E6-A22A49A2E0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="create" sheetId="5" r:id="rId1"/>
     <sheet name="postdata" sheetId="2" r:id="rId2"/>
-    <sheet name="putdata" sheetId="3" r:id="rId3"/>
+    <sheet name="putdataId" sheetId="3" r:id="rId3"/>
+    <sheet name="putdataName" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>programName</t>
   </si>
@@ -41,34 +42,31 @@
     <t>Active</t>
   </si>
   <si>
-    <t>NinjaSparkSDET1</t>
-  </si>
-  <si>
     <t>Learn API</t>
   </si>
   <si>
     <t>API Testing Eclipse</t>
   </si>
   <si>
-    <t>API Testing cucumber</t>
-  </si>
-  <si>
-    <t>NinjaSparkCin221</t>
-  </si>
-  <si>
-    <t>NinjaSparkCin231</t>
-  </si>
-  <si>
-    <t>NinjaSparrree</t>
-  </si>
-  <si>
-    <t>NinjaDiiiee</t>
-  </si>
-  <si>
-    <t>Learn Automation</t>
-  </si>
-  <si>
-    <t>Learn API Test</t>
+    <t>Learn Automation Numpy Ninja</t>
+  </si>
+  <si>
+    <t>SDET Numpy Ninja</t>
+  </si>
+  <si>
+    <t>NinjaSparkSDET_Team9_10001</t>
+  </si>
+  <si>
+    <t>NinjaSparkTeam9_SDET_10001</t>
+  </si>
+  <si>
+    <t>NinjaSparkSDET111</t>
+  </si>
+  <si>
+    <t>NinjaSpark200111</t>
+  </si>
+  <si>
+    <t>API  cucumberr</t>
   </si>
 </sst>
 </file>
@@ -433,10 +431,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBF458C-3F05-453B-A50C-3F22DDDB678E}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D934DE-7C8E-4ABF-853C-4DAC70642562}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,24 +531,12 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -500,69 +544,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D934DE-7C8E-4ABF-853C-4DAC70642562}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7933EB-B12C-4508-B919-C5C7CBB0B968}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,28 +572,55 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279D079B-8CEF-4555-970A-B94E475C5E47}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>